<commit_message>
updated list of chips
also added a couple of data sheets
</commit_message>
<xml_diff>
--- a/robot.xlsx
+++ b/robot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrork1/Documents/Development/cyberguard-sr2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE8FA080-A081-F340-8350-616E52A4C829}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEBA9D8-0CC1-8A46-A85D-C039FE0DB650}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25680" yWindow="4880" windowWidth="21440" windowHeight="17440" activeTab="3" xr2:uid="{B1C0CE19-338F-8947-AB7C-047B783EFFB9}"/>
+    <workbookView xWindow="28120" yWindow="2100" windowWidth="21440" windowHeight="17440" activeTab="3" xr2:uid="{B1C0CE19-338F-8947-AB7C-047B783EFFB9}"/>
   </bookViews>
   <sheets>
     <sheet name="PORTS" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="154">
   <si>
     <t>F0</t>
   </si>
@@ -374,6 +374,123 @@
   </si>
   <si>
     <t>8000-9FFF</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/uln2803a.pdf?ts=1645366810061&amp;ref_url=https%253A%252F%252Fwww.google.com%252F</t>
+  </si>
+  <si>
+    <t>uln2803a</t>
+  </si>
+  <si>
+    <t>DarlingtonTransistor Arrays</t>
+  </si>
+  <si>
+    <t>sn74hc259n</t>
+  </si>
+  <si>
+    <t>sn74hc02n</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>Motorola</t>
+  </si>
+  <si>
+    <t>ADC0808N</t>
+  </si>
+  <si>
+    <t>Ti</t>
+  </si>
+  <si>
+    <t>SN74HC74N</t>
+  </si>
+  <si>
+    <t>SN74HC02N</t>
+  </si>
+  <si>
+    <t>LM324N</t>
+  </si>
+  <si>
+    <t>https://pdf1.alldatasheet.com/datasheet-pdf/view/22756/STMICROELECTRONICS/LM324N.html</t>
+  </si>
+  <si>
+    <t>mc14516bcp</t>
+  </si>
+  <si>
+    <t>MC74HC7266N</t>
+  </si>
+  <si>
+    <t>MC74HC14</t>
+  </si>
+  <si>
+    <t>SN74HC20N</t>
+  </si>
+  <si>
+    <t>SN74HC138N</t>
+  </si>
+  <si>
+    <t>MC14516BCP</t>
+  </si>
+  <si>
+    <t>MM14516BCN</t>
+  </si>
+  <si>
+    <t>SN74HC573N</t>
+  </si>
+  <si>
+    <t>74HC573</t>
+  </si>
+  <si>
+    <t>MC74HC08</t>
+  </si>
+  <si>
+    <t>SN74HC03N</t>
+  </si>
+  <si>
+    <t>SN74HC04N</t>
+  </si>
+  <si>
+    <t>Toshiba</t>
+  </si>
+  <si>
+    <t>TMPZ84C00AP</t>
+  </si>
+  <si>
+    <t>MCM6064P12</t>
+  </si>
+  <si>
+    <t>TMS 27C64-IJL</t>
+  </si>
+  <si>
+    <t>Zilog</t>
+  </si>
+  <si>
+    <t>Z84C3006PEC</t>
+  </si>
+  <si>
+    <t>Z80 CTC</t>
+  </si>
+  <si>
+    <t>Z84C4004PEC</t>
+  </si>
+  <si>
+    <t>Z80 SI0/0</t>
+  </si>
+  <si>
+    <t>SN74HC157N</t>
+  </si>
+  <si>
+    <t>SN74HC4060N</t>
+  </si>
+  <si>
+    <t>MC1489P</t>
+  </si>
+  <si>
+    <t>MC1488P</t>
   </si>
 </sst>
 </file>
@@ -383,7 +500,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -401,6 +518,14 @@
       <i/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -429,10 +554,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -448,8 +574,10 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1379,7 +1507,7 @@
   <dimension ref="A1:L65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
@@ -1985,228 +2113,493 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032DEE3F-8985-B643-ACD2-B7C894C9627B}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>141</v>
+      </c>
+      <c r="C32" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>121</v>
+      </c>
+      <c r="C34" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" t="s">
+        <v>146</v>
+      </c>
+      <c r="D36" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>145</v>
+      </c>
+      <c r="C37" t="s">
+        <v>148</v>
+      </c>
+      <c r="D37" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>38</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>121</v>
+      </c>
+      <c r="C38" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>121</v>
+      </c>
+      <c r="C39" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>122</v>
+      </c>
+      <c r="C40" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>42</v>
       </c>
+      <c r="B42" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" t="s">
+        <v>152</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E1" r:id="rId1" xr:uid="{6E3BAECD-BC03-574F-8CC8-E16354CE2625}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
finished gathering datasheets for mainboard
</commit_message>
<xml_diff>
--- a/robot.xlsx
+++ b/robot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrork1/Documents/Development/cyberguard-sr2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6794C9BB-7E5F-9E48-B135-EAAEF31E3AD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FF2C51-FC9B-7B4C-86A2-585917BD41D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28120" yWindow="2100" windowWidth="21440" windowHeight="17440" activeTab="1" xr2:uid="{B1C0CE19-338F-8947-AB7C-047B783EFFB9}"/>
+    <workbookView xWindow="24500" yWindow="5760" windowWidth="25560" windowHeight="17440" activeTab="1" xr2:uid="{B1C0CE19-338F-8947-AB7C-047B783EFFB9}"/>
   </bookViews>
   <sheets>
     <sheet name="PORTS" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,11 @@
     <sheet name="MEMORY MAP" sheetId="5" r:id="rId3"/>
     <sheet name="CHIPS" sheetId="4" r:id="rId4"/>
     <sheet name="OUT 1" sheetId="1" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CHIPS!$C$1:$C$44</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="163">
   <si>
     <t>F0</t>
   </si>
@@ -196,9 +200,6 @@
     <t>16 - 74hc139</t>
   </si>
   <si>
-    <t>74hc139</t>
-  </si>
-  <si>
     <t>33 - A3</t>
   </si>
   <si>
@@ -379,18 +380,9 @@
     <t>https://www.ti.com/lit/ds/symlink/uln2803a.pdf?ts=1645366810061&amp;ref_url=https%253A%252F%252Fwww.google.com%252F</t>
   </si>
   <si>
-    <t>uln2803a</t>
-  </si>
-  <si>
     <t>DarlingtonTransistor Arrays</t>
   </si>
   <si>
-    <t>sn74hc259n</t>
-  </si>
-  <si>
-    <t>sn74hc02n</t>
-  </si>
-  <si>
     <t>ST</t>
   </si>
   <si>
@@ -418,9 +410,6 @@
     <t>https://pdf1.alldatasheet.com/datasheet-pdf/view/22756/STMICROELECTRONICS/LM324N.html</t>
   </si>
   <si>
-    <t>mc14516bcp</t>
-  </si>
-  <si>
     <t>MC74HC7266N</t>
   </si>
   <si>
@@ -436,15 +425,9 @@
     <t>MC14516BCP</t>
   </si>
   <si>
-    <t>MM14516BCN</t>
-  </si>
-  <si>
     <t>SN74HC573N</t>
   </si>
   <si>
-    <t>74HC573</t>
-  </si>
-  <si>
     <t>MC74HC08</t>
   </si>
   <si>
@@ -497,6 +480,48 @@
   </si>
   <si>
     <t>8-BIT ADDRESSABLE LATCHES</t>
+  </si>
+  <si>
+    <t>https://pdf1.alldatasheet.com/datasheet-pdf/view/8097/NSC/ADC0808.html</t>
+  </si>
+  <si>
+    <t>8-Bit μP Compatible A/D Converters with 8-ChannelMultiplexer</t>
+  </si>
+  <si>
+    <t>ULN2803A</t>
+  </si>
+  <si>
+    <t>SN74HC259N</t>
+  </si>
+  <si>
+    <t>SN74HC139</t>
+  </si>
+  <si>
+    <t>SN74HC573</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>CD4516BCN</t>
+  </si>
+  <si>
+    <t>p3</t>
+  </si>
+  <si>
+    <t>From chip</t>
+  </si>
+  <si>
+    <t>to chip</t>
+  </si>
+  <si>
+    <t>to pin</t>
+  </si>
+  <si>
+    <t>from pin</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -899,7 +924,7 @@
   <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView zoomScale="118" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -915,52 +940,52 @@
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="U1" s="8" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
@@ -1000,26 +1025,26 @@
         <v>0</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q2" s="3"/>
       <c r="R2" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -1056,29 +1081,29 @@
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q3" s="10"/>
       <c r="R3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U3" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -1115,29 +1140,29 @@
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -1174,29 +1199,29 @@
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q5" s="3"/>
       <c r="R5" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U5" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -1233,29 +1258,29 @@
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q6" s="3"/>
       <c r="R6" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T6" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -1292,29 +1317,29 @@
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P7" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q7" s="10"/>
       <c r="R7" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -1351,29 +1376,29 @@
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q8" s="10"/>
       <c r="R8" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
@@ -1410,29 +1435,29 @@
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q9" s="10"/>
       <c r="R9" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U9" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
@@ -1469,29 +1494,29 @@
       </c>
       <c r="L10" s="3"/>
       <c r="M10" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q10" s="10"/>
       <c r="R10" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T10" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U10" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
@@ -1513,8 +1538,8 @@
   <dimension ref="A1:L65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D64" sqref="D64"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A52" sqref="A52:XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1533,10 +1558,10 @@
         <v>51</v>
       </c>
       <c r="D1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" t="s">
         <v>101</v>
-      </c>
-      <c r="E1" t="s">
-        <v>102</v>
       </c>
       <c r="F1" t="s">
         <v>52</v>
@@ -1554,7 +1579,7 @@
         <v>54</v>
       </c>
       <c r="K1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L1">
         <v>14</v>
@@ -1817,10 +1842,10 @@
     </row>
     <row r="35" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I35" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -1903,10 +1928,10 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
@@ -1936,119 +1961,119 @@
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
+        <v>59</v>
+      </c>
+      <c r="J53" t="s">
         <v>60</v>
-      </c>
-      <c r="J53" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
+        <v>65</v>
+      </c>
+      <c r="J54" t="s">
         <v>66</v>
-      </c>
-      <c r="J54" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
+        <v>67</v>
+      </c>
+      <c r="K55" t="s">
         <v>68</v>
-      </c>
-      <c r="K55" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K57" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.2">
       <c r="G58" t="s">
+        <v>72</v>
+      </c>
+      <c r="K58" t="s">
         <v>73</v>
-      </c>
-      <c r="K58" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.2">
       <c r="F59" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K59" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C60" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K60" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
+        <v>95</v>
+      </c>
+      <c r="K61" t="s">
         <v>96</v>
-      </c>
-      <c r="K61" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K62" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K63" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D64" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K64" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="65" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E65" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K65" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2074,42 +2099,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2119,498 +2144,636 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032DEE3F-8985-B643-ACD2-B7C894C9627B}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.6640625" customWidth="1"/>
+    <col min="5" max="5" width="53.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="E1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>118</v>
       </c>
-      <c r="D2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>121</v>
-      </c>
       <c r="C3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="D3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="D4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="D5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="D6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="D7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="D8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+      <c r="D9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="D10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="D11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+      <c r="D12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>13</v>
       </c>
       <c r="B13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>156</v>
+      </c>
+      <c r="D17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" t="s">
         <v>122</v>
       </c>
-      <c r="C13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="D18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" t="s">
+        <v>133</v>
+      </c>
+      <c r="D21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>38</v>
+      </c>
+      <c r="B24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" t="s">
+        <v>143</v>
+      </c>
+      <c r="D24" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" t="s">
+        <v>155</v>
+      </c>
+      <c r="E26" t="s">
+        <v>148</v>
+      </c>
+      <c r="F26" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>39</v>
+      </c>
+      <c r="B27" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" t="s">
+        <v>144</v>
+      </c>
+      <c r="D27" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" t="s">
+        <v>154</v>
+      </c>
+      <c r="D28" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" t="s">
+        <v>130</v>
+      </c>
+      <c r="D29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>21</v>
+      </c>
+      <c r="B30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" t="s">
+        <v>130</v>
+      </c>
+      <c r="D30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C31" t="s">
         <v>121</v>
       </c>
-      <c r="C14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="D31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C32" t="s">
         <v>121</v>
       </c>
-      <c r="C15" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>16</v>
-      </c>
-      <c r="C16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>122</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>25</v>
+      </c>
+      <c r="B33" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>26</v>
+      </c>
+      <c r="B34" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>27</v>
+      </c>
+      <c r="B35" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>122</v>
-      </c>
-      <c r="C18" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="C37" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>121</v>
-      </c>
-      <c r="C20" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>121</v>
-      </c>
-      <c r="C21" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>122</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="D37" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>34</v>
+      </c>
+      <c r="B38" t="s">
+        <v>117</v>
+      </c>
+      <c r="C38" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>23</v>
-      </c>
-      <c r="B23" t="s">
-        <v>122</v>
-      </c>
-      <c r="C23" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>122</v>
-      </c>
-      <c r="C24" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>25</v>
-      </c>
-      <c r="B25" t="s">
-        <v>121</v>
-      </c>
-      <c r="C25" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>26</v>
-      </c>
-      <c r="B26" t="s">
-        <v>121</v>
-      </c>
-      <c r="C26" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>27</v>
-      </c>
-      <c r="B27" t="s">
-        <v>121</v>
-      </c>
-      <c r="C27" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>28</v>
-      </c>
-      <c r="B28" t="s">
-        <v>122</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="D38" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>35</v>
+      </c>
+      <c r="B39" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" t="s">
+        <v>137</v>
+      </c>
+      <c r="D39" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" t="s">
+        <v>151</v>
+      </c>
+      <c r="D40" t="s">
+        <v>155</v>
+      </c>
+      <c r="E40" t="s">
+        <v>115</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>36</v>
+      </c>
+      <c r="B41" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>29</v>
-      </c>
-      <c r="B29" t="s">
-        <v>121</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="C41" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>30</v>
-      </c>
-      <c r="B30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>31</v>
-      </c>
-      <c r="B31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="D41" t="s">
+        <v>155</v>
+      </c>
+      <c r="E41" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>32</v>
-      </c>
-      <c r="B32" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>37</v>
+      </c>
+      <c r="B42" t="s">
+        <v>138</v>
+      </c>
+      <c r="C42" t="s">
         <v>141</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D42" t="s">
+        <v>155</v>
+      </c>
+      <c r="E42" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>33</v>
-      </c>
-      <c r="B33" t="s">
-        <v>122</v>
-      </c>
-      <c r="C33" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>34</v>
-      </c>
-      <c r="B34" t="s">
-        <v>121</v>
-      </c>
-      <c r="C34" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>35</v>
-      </c>
-      <c r="B35" t="s">
-        <v>121</v>
-      </c>
-      <c r="C35" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>36</v>
-      </c>
-      <c r="B36" t="s">
-        <v>145</v>
-      </c>
-      <c r="C36" t="s">
-        <v>146</v>
-      </c>
-      <c r="D36" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>37</v>
-      </c>
-      <c r="B37" t="s">
-        <v>145</v>
-      </c>
-      <c r="C37" t="s">
-        <v>148</v>
-      </c>
-      <c r="D37" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>38</v>
-      </c>
-      <c r="B38" t="s">
-        <v>121</v>
-      </c>
-      <c r="C38" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>39</v>
-      </c>
-      <c r="B39" t="s">
-        <v>121</v>
-      </c>
-      <c r="C39" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>40</v>
-      </c>
-      <c r="B40" t="s">
-        <v>122</v>
-      </c>
-      <c r="C40" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>41</v>
-      </c>
-      <c r="B41" t="s">
-        <v>122</v>
-      </c>
-      <c r="C41" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>42</v>
-      </c>
-      <c r="B42" t="s">
-        <v>122</v>
-      </c>
-      <c r="C42" t="s">
-        <v>152</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="C1:C44" xr:uid="{58B52DAE-4C08-F54F-8949-125CF7ACCC05}"/>
+  <sortState ref="A1:F43">
+    <sortCondition ref="C1"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="E1" r:id="rId1" xr:uid="{6E3BAECD-BC03-574F-8CC8-E16354CE2625}"/>
+    <hyperlink ref="F40" r:id="rId1" xr:uid="{6E3BAECD-BC03-574F-8CC8-E16354CE2625}"/>
+    <hyperlink ref="F1" r:id="rId2" xr:uid="{FC5363BE-C302-1043-8F2C-45B55E7FA1ED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2903,4 +3066,117 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D57B502-468F-EE4C-9DB0-E38D3298CC0F}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>32</v>
+      </c>
+      <c r="D7">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>